<commit_message>
Stated making OOP version of DD20parser
</commit_message>
<xml_diff>
--- a/tests/valid-testdata/Limits_other.xlsx
+++ b/tests/valid-testdata/Limits_other.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="Denne_projektmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/awi_energinet_dk/Documents/Skrivebord/Mock til DLR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/awi_energinet_dk/Documents/Skrivebord/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{10643D07-CD96-4B31-B7DB-5B011FEC6B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{038549F8-5B88-4F34-B66A-0B3D0451ED93}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{10643D07-CD96-4B31-B7DB-5B011FEC6B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5508F846-0848-4955-8196-CD5F7F1EE5FB}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="4560" windowWidth="31350" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7665" yWindow="465" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DD20Mapping" sheetId="12" r:id="rId1"/>
@@ -43,10 +43,10 @@
     <t>andet navn i ETS. Forkert model.</t>
   </si>
   <si>
-    <t>E_EEEV-FFF-1</t>
-  </si>
-  <si>
-    <t>E_EEE-FFF-1</t>
+    <t>E_EEE-FFF_1</t>
+  </si>
+  <si>
+    <t>E_EEEV-FFF_1</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="M3" sqref="M3:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,10 +484,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Feature/dd20 format change (#9)
Major change to create base code for the repo. First version which is production ready, however several issues are opened and will be adressed in future versions.
</commit_message>
<xml_diff>
--- a/tests/valid-testdata/Limits_other.xlsx
+++ b/tests/valid-testdata/Limits_other.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/awi_energinet_dk/Documents/Skrivebord/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10643D07-CD96-4B31-B7DB-5B011FEC6B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{10643D07-CD96-4B31-B7DB-5B011FEC6B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5508F846-0848-4955-8196-CD5F7F1EE5FB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7665" yWindow="465" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DD20Mapping" sheetId="12" r:id="rId1"/>
@@ -43,10 +43,10 @@
     <t>andet navn i ETS. Forkert model.</t>
   </si>
   <si>
-    <t>E_GGG-HHH</t>
-  </si>
-  <si>
-    <t>E_GGGV-HHH</t>
+    <t>E_EEE-FFF_1</t>
+  </si>
+  <si>
+    <t>E_EEEV-FFF_1</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
+      <selection activeCell="M3" sqref="M3:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>